<commit_message>
Updating the neoplasms categories
</commit_message>
<xml_diff>
--- a/dat/10-cod-list/cod.xlsx
+++ b/dat/10-cod-list/cod.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\gits\new\bhump\dat\10-cod-list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C090E7C1-DF2B-4A7F-A91D-F87DA71A2924}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B70881E4-65C5-4DF1-86C7-C102F256E2F4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3758,8 +3758,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -4115,10 +4116,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D1073"/>
+  <dimension ref="A1:E1073"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+    <sheetView tabSelected="1" topLeftCell="A1027" workbookViewId="0">
+      <selection activeCell="E919" sqref="E919"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4840,7 +4841,7 @@
         <v>69</v>
       </c>
       <c r="B90" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
@@ -9894,7 +9895,7 @@
         <v>603</v>
       </c>
       <c r="B721" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
     </row>
     <row r="722" spans="1:2" x14ac:dyDescent="0.25">
@@ -9902,7 +9903,7 @@
         <v>604</v>
       </c>
       <c r="B722" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
     </row>
     <row r="723" spans="1:2" x14ac:dyDescent="0.25">
@@ -9910,7 +9911,7 @@
         <v>605</v>
       </c>
       <c r="B723" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
     </row>
     <row r="724" spans="1:2" x14ac:dyDescent="0.25">
@@ -9918,7 +9919,7 @@
         <v>606</v>
       </c>
       <c r="B724" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
     </row>
     <row r="725" spans="1:2" x14ac:dyDescent="0.25">
@@ -9926,7 +9927,7 @@
         <v>607</v>
       </c>
       <c r="B725" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
     </row>
     <row r="726" spans="1:2" x14ac:dyDescent="0.25">
@@ -9934,7 +9935,7 @@
         <v>930</v>
       </c>
       <c r="B726" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
     </row>
     <row r="727" spans="1:2" x14ac:dyDescent="0.25">
@@ -9942,7 +9943,7 @@
         <v>608</v>
       </c>
       <c r="B727" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
     </row>
     <row r="728" spans="1:2" x14ac:dyDescent="0.25">
@@ -9950,7 +9951,7 @@
         <v>609</v>
       </c>
       <c r="B728" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
     </row>
     <row r="729" spans="1:2" x14ac:dyDescent="0.25">
@@ -9958,7 +9959,7 @@
         <v>610</v>
       </c>
       <c r="B729" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
     </row>
     <row r="730" spans="1:2" x14ac:dyDescent="0.25">
@@ -9966,7 +9967,7 @@
         <v>611</v>
       </c>
       <c r="B730" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
     </row>
     <row r="731" spans="1:2" x14ac:dyDescent="0.25">
@@ -9974,7 +9975,7 @@
         <v>612</v>
       </c>
       <c r="B731" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
     </row>
     <row r="732" spans="1:2" x14ac:dyDescent="0.25">
@@ -9982,7 +9983,7 @@
         <v>613</v>
       </c>
       <c r="B732" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
     </row>
     <row r="733" spans="1:2" x14ac:dyDescent="0.25">
@@ -9990,7 +9991,7 @@
         <v>931</v>
       </c>
       <c r="B733" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
     </row>
     <row r="734" spans="1:2" x14ac:dyDescent="0.25">
@@ -9998,7 +9999,7 @@
         <v>614</v>
       </c>
       <c r="B734" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
     </row>
     <row r="735" spans="1:2" x14ac:dyDescent="0.25">
@@ -10006,7 +10007,7 @@
         <v>615</v>
       </c>
       <c r="B735" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
     </row>
     <row r="736" spans="1:2" x14ac:dyDescent="0.25">
@@ -10014,7 +10015,7 @@
         <v>932</v>
       </c>
       <c r="B736" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
     </row>
     <row r="737" spans="1:2" x14ac:dyDescent="0.25">
@@ -10022,7 +10023,7 @@
         <v>616</v>
       </c>
       <c r="B737" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
     </row>
     <row r="738" spans="1:2" x14ac:dyDescent="0.25">
@@ -10030,7 +10031,7 @@
         <v>617</v>
       </c>
       <c r="B738" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
     </row>
     <row r="739" spans="1:2" x14ac:dyDescent="0.25">
@@ -10038,7 +10039,7 @@
         <v>618</v>
       </c>
       <c r="B739" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
     </row>
     <row r="740" spans="1:2" x14ac:dyDescent="0.25">
@@ -10046,7 +10047,7 @@
         <v>619</v>
       </c>
       <c r="B740" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
     </row>
     <row r="741" spans="1:2" x14ac:dyDescent="0.25">
@@ -10054,7 +10055,7 @@
         <v>620</v>
       </c>
       <c r="B741" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
     </row>
     <row r="742" spans="1:2" x14ac:dyDescent="0.25">
@@ -10062,7 +10063,7 @@
         <v>621</v>
       </c>
       <c r="B742" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
     </row>
     <row r="743" spans="1:2" x14ac:dyDescent="0.25">
@@ -10070,7 +10071,7 @@
         <v>622</v>
       </c>
       <c r="B743" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
     </row>
     <row r="744" spans="1:2" x14ac:dyDescent="0.25">
@@ -10078,7 +10079,7 @@
         <v>623</v>
       </c>
       <c r="B744" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
     </row>
     <row r="745" spans="1:2" x14ac:dyDescent="0.25">
@@ -10086,7 +10087,7 @@
         <v>624</v>
       </c>
       <c r="B745" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
     </row>
     <row r="746" spans="1:2" x14ac:dyDescent="0.25">
@@ -10094,7 +10095,7 @@
         <v>625</v>
       </c>
       <c r="B746" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
     </row>
     <row r="747" spans="1:2" x14ac:dyDescent="0.25">
@@ -10102,7 +10103,7 @@
         <v>626</v>
       </c>
       <c r="B747" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
     </row>
     <row r="748" spans="1:2" x14ac:dyDescent="0.25">
@@ -10110,7 +10111,7 @@
         <v>627</v>
       </c>
       <c r="B748" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
     </row>
     <row r="749" spans="1:2" x14ac:dyDescent="0.25">
@@ -10118,7 +10119,7 @@
         <v>628</v>
       </c>
       <c r="B749" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
     </row>
     <row r="750" spans="1:2" x14ac:dyDescent="0.25">
@@ -10126,7 +10127,7 @@
         <v>933</v>
       </c>
       <c r="B750" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
     </row>
     <row r="751" spans="1:2" x14ac:dyDescent="0.25">
@@ -10134,7 +10135,7 @@
         <v>629</v>
       </c>
       <c r="B751" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
     </row>
     <row r="752" spans="1:2" x14ac:dyDescent="0.25">
@@ -10142,7 +10143,7 @@
         <v>630</v>
       </c>
       <c r="B752" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
     </row>
     <row r="753" spans="1:2" x14ac:dyDescent="0.25">
@@ -10150,7 +10151,7 @@
         <v>631</v>
       </c>
       <c r="B753" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
     </row>
     <row r="754" spans="1:2" x14ac:dyDescent="0.25">
@@ -10158,7 +10159,7 @@
         <v>632</v>
       </c>
       <c r="B754" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
     </row>
     <row r="755" spans="1:2" x14ac:dyDescent="0.25">
@@ -10166,7 +10167,7 @@
         <v>633</v>
       </c>
       <c r="B755" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
     </row>
     <row r="756" spans="1:2" x14ac:dyDescent="0.25">
@@ -10174,7 +10175,7 @@
         <v>634</v>
       </c>
       <c r="B756" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
     </row>
     <row r="757" spans="1:2" x14ac:dyDescent="0.25">
@@ -10182,7 +10183,7 @@
         <v>635</v>
       </c>
       <c r="B757" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
     </row>
     <row r="758" spans="1:2" x14ac:dyDescent="0.25">
@@ -10190,7 +10191,7 @@
         <v>636</v>
       </c>
       <c r="B758" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
     </row>
     <row r="759" spans="1:2" x14ac:dyDescent="0.25">
@@ -10198,7 +10199,7 @@
         <v>637</v>
       </c>
       <c r="B759" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
     </row>
     <row r="760" spans="1:2" x14ac:dyDescent="0.25">
@@ -10206,7 +10207,7 @@
         <v>638</v>
       </c>
       <c r="B760" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
     </row>
     <row r="761" spans="1:2" x14ac:dyDescent="0.25">
@@ -10214,7 +10215,7 @@
         <v>639</v>
       </c>
       <c r="B761" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
     </row>
     <row r="762" spans="1:2" x14ac:dyDescent="0.25">
@@ -10222,7 +10223,7 @@
         <v>640</v>
       </c>
       <c r="B762" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
     </row>
     <row r="763" spans="1:2" x14ac:dyDescent="0.25">
@@ -10230,7 +10231,7 @@
         <v>641</v>
       </c>
       <c r="B763" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
     </row>
     <row r="764" spans="1:2" x14ac:dyDescent="0.25">
@@ -10238,7 +10239,7 @@
         <v>642</v>
       </c>
       <c r="B764" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
     </row>
     <row r="765" spans="1:2" x14ac:dyDescent="0.25">
@@ -10246,7 +10247,7 @@
         <v>643</v>
       </c>
       <c r="B765" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
     </row>
     <row r="766" spans="1:2" x14ac:dyDescent="0.25">
@@ -10254,7 +10255,7 @@
         <v>934</v>
       </c>
       <c r="B766" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
     </row>
     <row r="767" spans="1:2" x14ac:dyDescent="0.25">
@@ -10262,7 +10263,7 @@
         <v>644</v>
       </c>
       <c r="B767" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
     </row>
     <row r="768" spans="1:2" x14ac:dyDescent="0.25">
@@ -10270,7 +10271,7 @@
         <v>645</v>
       </c>
       <c r="B768" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
     </row>
     <row r="769" spans="1:2" x14ac:dyDescent="0.25">
@@ -10278,7 +10279,7 @@
         <v>646</v>
       </c>
       <c r="B769" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
     </row>
     <row r="770" spans="1:2" x14ac:dyDescent="0.25">
@@ -10286,7 +10287,7 @@
         <v>647</v>
       </c>
       <c r="B770" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
     </row>
     <row r="771" spans="1:2" x14ac:dyDescent="0.25">
@@ -10294,7 +10295,7 @@
         <v>648</v>
       </c>
       <c r="B771" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
     </row>
     <row r="772" spans="1:2" x14ac:dyDescent="0.25">
@@ -10302,7 +10303,7 @@
         <v>935</v>
       </c>
       <c r="B772" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
     </row>
     <row r="773" spans="1:2" x14ac:dyDescent="0.25">
@@ -10310,7 +10311,7 @@
         <v>649</v>
       </c>
       <c r="B773" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
     </row>
     <row r="774" spans="1:2" x14ac:dyDescent="0.25">
@@ -10318,7 +10319,7 @@
         <v>650</v>
       </c>
       <c r="B774" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
     </row>
     <row r="775" spans="1:2" x14ac:dyDescent="0.25">
@@ -10326,7 +10327,7 @@
         <v>651</v>
       </c>
       <c r="B775" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
     </row>
     <row r="776" spans="1:2" x14ac:dyDescent="0.25">
@@ -10657,7 +10658,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="817" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="817" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A817" t="s">
         <v>691</v>
       </c>
@@ -10665,7 +10666,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="818" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="818" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A818" t="s">
         <v>692</v>
       </c>
@@ -10673,7 +10674,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="819" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="819" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A819" t="s">
         <v>937</v>
       </c>
@@ -10681,7 +10682,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="820" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="820" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A820" t="s">
         <v>693</v>
       </c>
@@ -10689,7 +10690,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="821" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="821" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A821" t="s">
         <v>1077</v>
       </c>
@@ -10697,71 +10698,72 @@
         <v>49</v>
       </c>
     </row>
-    <row r="822" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="822" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A822" t="s">
         <v>694</v>
       </c>
       <c r="B822" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="823" spans="1:2" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="823" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A823" t="s">
         <v>695</v>
       </c>
       <c r="B823" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="824" spans="1:2" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="824" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A824" t="s">
         <v>696</v>
       </c>
       <c r="B824" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="825" spans="1:2" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="825" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A825" t="s">
         <v>697</v>
       </c>
       <c r="B825" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="826" spans="1:2" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="826" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A826" t="s">
         <v>938</v>
       </c>
       <c r="B826" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="827" spans="1:2" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="827" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A827" t="s">
         <v>1078</v>
       </c>
       <c r="B827" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="828" spans="1:2" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="828" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A828" t="s">
         <v>698</v>
       </c>
       <c r="B828" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="829" spans="1:2" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="829" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A829" t="s">
         <v>699</v>
       </c>
       <c r="B829" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="830" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E829" s="1"/>
+    </row>
+    <row r="830" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A830" t="s">
         <v>700</v>
       </c>
@@ -10769,7 +10771,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="831" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="831" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A831" t="s">
         <v>701</v>
       </c>
@@ -10777,7 +10779,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="832" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="832" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A832" t="s">
         <v>702</v>
       </c>
@@ -10950,7 +10952,7 @@
         <v>720</v>
       </c>
       <c r="B853" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
     </row>
     <row r="854" spans="1:2" x14ac:dyDescent="0.25">
@@ -10958,7 +10960,7 @@
         <v>721</v>
       </c>
       <c r="B854" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
     </row>
     <row r="855" spans="1:2" x14ac:dyDescent="0.25">
@@ -10966,7 +10968,7 @@
         <v>722</v>
       </c>
       <c r="B855" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
     </row>
     <row r="856" spans="1:2" x14ac:dyDescent="0.25">
@@ -11030,7 +11032,7 @@
         <v>730</v>
       </c>
       <c r="B863" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
     </row>
     <row r="864" spans="1:2" x14ac:dyDescent="0.25">
@@ -11038,7 +11040,7 @@
         <v>731</v>
       </c>
       <c r="B864" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
     </row>
     <row r="865" spans="1:2" x14ac:dyDescent="0.25">
@@ -11046,7 +11048,7 @@
         <v>732</v>
       </c>
       <c r="B865" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
     </row>
     <row r="866" spans="1:2" x14ac:dyDescent="0.25">
@@ -11054,7 +11056,7 @@
         <v>733</v>
       </c>
       <c r="B866" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
     </row>
     <row r="867" spans="1:2" x14ac:dyDescent="0.25">
@@ -11062,7 +11064,7 @@
         <v>734</v>
       </c>
       <c r="B867" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
     </row>
     <row r="868" spans="1:2" x14ac:dyDescent="0.25">
@@ -11086,7 +11088,7 @@
         <v>737</v>
       </c>
       <c r="B870" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
     </row>
     <row r="871" spans="1:2" x14ac:dyDescent="0.25">
@@ -11094,7 +11096,7 @@
         <v>738</v>
       </c>
       <c r="B871" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
     </row>
     <row r="872" spans="1:2" x14ac:dyDescent="0.25">
@@ -11102,7 +11104,7 @@
         <v>739</v>
       </c>
       <c r="B872" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
     </row>
     <row r="873" spans="1:2" x14ac:dyDescent="0.25">
@@ -11110,7 +11112,7 @@
         <v>740</v>
       </c>
       <c r="B873" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
     </row>
     <row r="874" spans="1:2" x14ac:dyDescent="0.25">
@@ -11118,7 +11120,7 @@
         <v>741</v>
       </c>
       <c r="B874" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
     </row>
     <row r="875" spans="1:2" x14ac:dyDescent="0.25">
@@ -11126,7 +11128,7 @@
         <v>742</v>
       </c>
       <c r="B875" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
     </row>
     <row r="876" spans="1:2" x14ac:dyDescent="0.25">
@@ -11134,7 +11136,7 @@
         <v>941</v>
       </c>
       <c r="B876" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
     </row>
     <row r="877" spans="1:2" x14ac:dyDescent="0.25">
@@ -11142,7 +11144,7 @@
         <v>743</v>
       </c>
       <c r="B877" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
     </row>
     <row r="878" spans="1:2" x14ac:dyDescent="0.25">
@@ -11254,7 +11256,7 @@
         <v>757</v>
       </c>
       <c r="B891" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
     </row>
     <row r="892" spans="1:2" x14ac:dyDescent="0.25">
@@ -11262,7 +11264,7 @@
         <v>942</v>
       </c>
       <c r="B892" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
     </row>
     <row r="893" spans="1:2" x14ac:dyDescent="0.25">
@@ -11270,7 +11272,7 @@
         <v>943</v>
       </c>
       <c r="B893" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
     </row>
     <row r="894" spans="1:2" x14ac:dyDescent="0.25">
@@ -11318,7 +11320,7 @@
         <v>762</v>
       </c>
       <c r="B899" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
     </row>
     <row r="900" spans="1:2" x14ac:dyDescent="0.25">
@@ -11326,7 +11328,7 @@
         <v>763</v>
       </c>
       <c r="B900" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
     </row>
     <row r="901" spans="1:2" x14ac:dyDescent="0.25">
@@ -11334,7 +11336,7 @@
         <v>764</v>
       </c>
       <c r="B901" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
     </row>
     <row r="902" spans="1:2" x14ac:dyDescent="0.25">
@@ -11342,7 +11344,7 @@
         <v>765</v>
       </c>
       <c r="B902" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
     </row>
     <row r="903" spans="1:2" x14ac:dyDescent="0.25">
@@ -11350,7 +11352,7 @@
         <v>945</v>
       </c>
       <c r="B903" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
     </row>
     <row r="904" spans="1:2" x14ac:dyDescent="0.25">
@@ -11358,7 +11360,7 @@
         <v>766</v>
       </c>
       <c r="B904" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
     </row>
     <row r="905" spans="1:2" x14ac:dyDescent="0.25">
@@ -11422,7 +11424,7 @@
         <v>774</v>
       </c>
       <c r="B912" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
     </row>
     <row r="913" spans="1:2" x14ac:dyDescent="0.25">
@@ -11430,7 +11432,7 @@
         <v>946</v>
       </c>
       <c r="B913" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
     </row>
     <row r="914" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
translation of comments on cod
</commit_message>
<xml_diff>
--- a/dat/10-cod-list/cod.xlsx
+++ b/dat/10-cod-list/cod.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\gits\new\bhump\dat\10-cod-list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B70881E4-65C5-4DF1-86C7-C102F256E2F4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{731B0355-68E0-49CA-AAF5-94B065E64E42}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2148" uniqueCount="1085">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2157" uniqueCount="1093">
   <si>
     <t>A022</t>
   </si>
@@ -3275,6 +3275,53 @@
   </si>
   <si>
     <t>cod_cat</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">#everything starts at treatable, only when it is really not treatable </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>and</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> chances are really high to die i am assigning untreatable</t>
+    </r>
+  </si>
+  <si>
+    <t># Malformations kidneys</t>
+  </si>
+  <si>
+    <t># Chromosomal malformations</t>
+  </si>
+  <si>
+    <t># Lymphoedema</t>
+  </si>
+  <si>
+    <t># Epidermolysis bullosa</t>
+  </si>
+  <si>
+    <t># Malformations respiratory system</t>
+  </si>
+  <si>
+    <t># Malformations heart</t>
+  </si>
+  <si>
+    <t># Malformations of brain and nervous system</t>
   </si>
 </sst>
 </file>
@@ -4116,10 +4163,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E1073"/>
+  <dimension ref="A1:F1073"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1027" workbookViewId="0">
-      <selection activeCell="E919" sqref="E919"/>
+    <sheetView tabSelected="1" topLeftCell="A438" workbookViewId="0">
+      <selection activeCell="E693" sqref="E693"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4508,7 +4555,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>39</v>
       </c>
@@ -4516,7 +4563,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>40</v>
       </c>
@@ -4524,7 +4571,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>1061</v>
       </c>
@@ -4532,7 +4579,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>41</v>
       </c>
@@ -4540,7 +4587,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>42</v>
       </c>
@@ -4548,7 +4595,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>43</v>
       </c>
@@ -4556,7 +4603,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>44</v>
       </c>
@@ -4564,7 +4611,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>45</v>
       </c>
@@ -4572,7 +4619,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>46</v>
       </c>
@@ -4580,7 +4627,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>864</v>
       </c>
@@ -4588,7 +4635,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>47</v>
       </c>
@@ -4596,7 +4643,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>1062</v>
       </c>
@@ -4604,7 +4651,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>959</v>
       </c>
@@ -4612,7 +4659,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>960</v>
       </c>
@@ -4620,7 +4667,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>961</v>
       </c>
@@ -4628,12 +4675,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>48</v>
       </c>
       <c r="B64" t="s">
         <v>49</v>
+      </c>
+      <c r="F64" t="s">
+        <v>1085</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
@@ -9634,7 +9684,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="689" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="689" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A689" t="s">
         <v>573</v>
       </c>
@@ -9642,7 +9692,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="690" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="690" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A690" t="s">
         <v>574</v>
       </c>
@@ -9650,7 +9700,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="691" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="691" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A691" t="s">
         <v>575</v>
       </c>
@@ -9658,15 +9708,18 @@
         <v>84</v>
       </c>
     </row>
-    <row r="692" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="692" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A692" t="s">
         <v>576</v>
       </c>
       <c r="B692" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="693" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E692" t="s">
+        <v>1092</v>
+      </c>
+    </row>
+    <row r="693" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A693" t="s">
         <v>577</v>
       </c>
@@ -9674,7 +9727,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="694" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="694" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A694" t="s">
         <v>578</v>
       </c>
@@ -9682,7 +9735,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="695" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="695" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A695" t="s">
         <v>579</v>
       </c>
@@ -9690,7 +9743,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="696" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="696" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A696" t="s">
         <v>580</v>
       </c>
@@ -9698,7 +9751,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="697" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="697" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A697" t="s">
         <v>1002</v>
       </c>
@@ -9706,7 +9759,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="698" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="698" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A698" t="s">
         <v>581</v>
       </c>
@@ -9714,7 +9767,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="699" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="699" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A699" t="s">
         <v>582</v>
       </c>
@@ -9722,7 +9775,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="700" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="700" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A700" t="s">
         <v>583</v>
       </c>
@@ -9730,7 +9783,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="701" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="701" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A701" t="s">
         <v>584</v>
       </c>
@@ -9738,7 +9791,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="702" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="702" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A702" t="s">
         <v>585</v>
       </c>
@@ -9746,7 +9799,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="703" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="703" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A703" t="s">
         <v>586</v>
       </c>
@@ -9754,7 +9807,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="704" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="704" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A704" t="s">
         <v>587</v>
       </c>
@@ -9890,15 +9943,18 @@
         <v>49</v>
       </c>
     </row>
-    <row r="721" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="721" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A721" t="s">
         <v>603</v>
       </c>
       <c r="B721" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="722" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E721" t="s">
+        <v>1091</v>
+      </c>
+    </row>
+    <row r="722" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A722" t="s">
         <v>604</v>
       </c>
@@ -9906,7 +9962,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="723" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="723" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A723" t="s">
         <v>605</v>
       </c>
@@ -9914,7 +9970,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="724" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="724" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A724" t="s">
         <v>606</v>
       </c>
@@ -9922,7 +9978,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="725" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="725" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A725" t="s">
         <v>607</v>
       </c>
@@ -9930,7 +9986,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="726" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="726" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A726" t="s">
         <v>930</v>
       </c>
@@ -9938,7 +9994,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="727" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="727" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A727" t="s">
         <v>608</v>
       </c>
@@ -9946,7 +10002,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="728" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="728" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A728" t="s">
         <v>609</v>
       </c>
@@ -9954,7 +10010,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="729" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="729" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A729" t="s">
         <v>610</v>
       </c>
@@ -9962,7 +10018,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="730" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="730" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A730" t="s">
         <v>611</v>
       </c>
@@ -9970,7 +10026,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="731" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="731" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A731" t="s">
         <v>612</v>
       </c>
@@ -9978,7 +10034,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="732" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="732" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A732" t="s">
         <v>613</v>
       </c>
@@ -9986,7 +10042,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="733" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="733" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A733" t="s">
         <v>931</v>
       </c>
@@ -9994,7 +10050,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="734" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="734" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A734" t="s">
         <v>614</v>
       </c>
@@ -10002,7 +10058,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="735" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="735" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A735" t="s">
         <v>615</v>
       </c>
@@ -10010,7 +10066,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="736" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="736" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A736" t="s">
         <v>932</v>
       </c>
@@ -10274,7 +10330,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="769" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="769" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A769" t="s">
         <v>646</v>
       </c>
@@ -10282,7 +10338,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="770" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="770" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A770" t="s">
         <v>647</v>
       </c>
@@ -10290,7 +10346,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="771" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="771" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A771" t="s">
         <v>648</v>
       </c>
@@ -10298,7 +10354,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="772" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="772" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A772" t="s">
         <v>935</v>
       </c>
@@ -10306,7 +10362,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="773" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="773" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A773" t="s">
         <v>649</v>
       </c>
@@ -10314,7 +10370,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="774" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="774" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A774" t="s">
         <v>650</v>
       </c>
@@ -10322,7 +10378,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="775" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="775" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A775" t="s">
         <v>651</v>
       </c>
@@ -10330,15 +10386,18 @@
         <v>70</v>
       </c>
     </row>
-    <row r="776" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="776" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A776" t="s">
         <v>652</v>
       </c>
       <c r="B776" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="777" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E776" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="777" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A777" t="s">
         <v>1076</v>
       </c>
@@ -10346,7 +10405,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="778" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="778" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A778" t="s">
         <v>653</v>
       </c>
@@ -10354,7 +10413,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="779" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="779" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A779" t="s">
         <v>654</v>
       </c>
@@ -10362,7 +10421,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="780" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="780" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A780" t="s">
         <v>655</v>
       </c>
@@ -10370,7 +10429,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="781" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="781" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A781" t="s">
         <v>656</v>
       </c>
@@ -10378,7 +10437,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="782" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="782" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A782" t="s">
         <v>657</v>
       </c>
@@ -10386,7 +10445,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="783" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="783" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A783" t="s">
         <v>658</v>
       </c>
@@ -10394,7 +10453,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="784" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="784" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A784" t="s">
         <v>659</v>
       </c>
@@ -10761,7 +10820,9 @@
       <c r="B829" t="s">
         <v>70</v>
       </c>
-      <c r="E829" s="1"/>
+      <c r="E829" s="1" t="s">
+        <v>1086</v>
+      </c>
     </row>
     <row r="830" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A830" t="s">
@@ -10787,7 +10848,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="833" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="833" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A833" t="s">
         <v>703</v>
       </c>
@@ -10795,7 +10856,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="834" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="834" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A834" t="s">
         <v>704</v>
       </c>
@@ -10803,7 +10864,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="835" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="835" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A835" t="s">
         <v>705</v>
       </c>
@@ -10811,7 +10872,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="836" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="836" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A836" t="s">
         <v>706</v>
       </c>
@@ -10819,7 +10880,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="837" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="837" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A837" t="s">
         <v>707</v>
       </c>
@@ -10827,7 +10888,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="838" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="838" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A838" t="s">
         <v>708</v>
       </c>
@@ -10835,7 +10896,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="839" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="839" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A839" t="s">
         <v>709</v>
       </c>
@@ -10843,7 +10904,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="840" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="840" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A840" t="s">
         <v>1079</v>
       </c>
@@ -10851,15 +10912,18 @@
         <v>49</v>
       </c>
     </row>
-    <row r="841" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="841" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A841" t="s">
         <v>939</v>
       </c>
       <c r="B841" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="842" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E841" s="1" t="s">
+        <v>1086</v>
+      </c>
+    </row>
+    <row r="842" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A842" t="s">
         <v>710</v>
       </c>
@@ -10867,7 +10931,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="843" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="843" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A843" t="s">
         <v>940</v>
       </c>
@@ -10875,7 +10939,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="844" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="844" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A844" t="s">
         <v>711</v>
       </c>
@@ -10883,7 +10947,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="845" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="845" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A845" t="s">
         <v>712</v>
       </c>
@@ -10891,7 +10955,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="846" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="846" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A846" t="s">
         <v>713</v>
       </c>
@@ -10899,7 +10963,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="847" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="847" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A847" t="s">
         <v>714</v>
       </c>
@@ -10907,7 +10971,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="848" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="848" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A848" t="s">
         <v>715</v>
       </c>
@@ -11171,7 +11235,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="881" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="881" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A881" t="s">
         <v>747</v>
       </c>
@@ -11179,7 +11243,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="882" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="882" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A882" t="s">
         <v>748</v>
       </c>
@@ -11187,7 +11251,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="883" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="883" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A883" t="s">
         <v>749</v>
       </c>
@@ -11195,7 +11259,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="884" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="884" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A884" t="s">
         <v>750</v>
       </c>
@@ -11203,7 +11267,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="885" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="885" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A885" t="s">
         <v>751</v>
       </c>
@@ -11211,7 +11275,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="886" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="886" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A886" t="s">
         <v>752</v>
       </c>
@@ -11219,7 +11283,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="887" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="887" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A887" t="s">
         <v>753</v>
       </c>
@@ -11227,7 +11291,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="888" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="888" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A888" t="s">
         <v>754</v>
       </c>
@@ -11235,7 +11299,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="889" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="889" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A889" t="s">
         <v>755</v>
       </c>
@@ -11243,7 +11307,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="890" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="890" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A890" t="s">
         <v>756</v>
       </c>
@@ -11251,7 +11315,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="891" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="891" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A891" t="s">
         <v>757</v>
       </c>
@@ -11259,7 +11323,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="892" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="892" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A892" t="s">
         <v>942</v>
       </c>
@@ -11267,7 +11331,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="893" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="893" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A893" t="s">
         <v>943</v>
       </c>
@@ -11275,15 +11339,18 @@
         <v>49</v>
       </c>
     </row>
-    <row r="894" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="894" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A894" t="s">
         <v>758</v>
       </c>
       <c r="B894" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="895" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E894" t="s">
+        <v>1089</v>
+      </c>
+    </row>
+    <row r="895" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A895" t="s">
         <v>759</v>
       </c>
@@ -11291,12 +11358,15 @@
         <v>70</v>
       </c>
     </row>
-    <row r="896" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="896" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A896" t="s">
         <v>760</v>
       </c>
       <c r="B896" t="s">
         <v>70</v>
+      </c>
+      <c r="E896" t="s">
+        <v>1088</v>
       </c>
     </row>
     <row r="897" spans="1:2" x14ac:dyDescent="0.25">
@@ -11427,7 +11497,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="913" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="913" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A913" t="s">
         <v>946</v>
       </c>
@@ -11435,7 +11505,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="914" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="914" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A914" t="s">
         <v>775</v>
       </c>
@@ -11443,7 +11513,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="915" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="915" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A915" t="s">
         <v>776</v>
       </c>
@@ -11451,7 +11521,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="916" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="916" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A916" t="s">
         <v>777</v>
       </c>
@@ -11459,7 +11529,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="917" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="917" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A917" t="s">
         <v>778</v>
       </c>
@@ -11467,7 +11537,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="918" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="918" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A918" t="s">
         <v>779</v>
       </c>
@@ -11475,15 +11545,18 @@
         <v>70</v>
       </c>
     </row>
-    <row r="919" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="919" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A919" t="s">
         <v>780</v>
       </c>
       <c r="B919" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="920" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E919" t="s">
+        <v>1087</v>
+      </c>
+    </row>
+    <row r="920" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A920" t="s">
         <v>781</v>
       </c>
@@ -11491,7 +11564,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="921" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="921" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A921" t="s">
         <v>782</v>
       </c>
@@ -11499,7 +11572,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="922" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="922" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A922" t="s">
         <v>783</v>
       </c>
@@ -11507,7 +11580,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="923" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="923" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A923" t="s">
         <v>784</v>
       </c>
@@ -11515,7 +11588,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="924" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="924" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A924" t="s">
         <v>785</v>
       </c>
@@ -11523,7 +11596,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="925" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="925" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A925" t="s">
         <v>786</v>
       </c>
@@ -11531,7 +11604,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="926" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="926" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A926" t="s">
         <v>787</v>
       </c>
@@ -11539,7 +11612,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="927" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="927" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A927" t="s">
         <v>788</v>
       </c>
@@ -11547,7 +11620,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="928" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="928" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A928" t="s">
         <v>947</v>
       </c>

</xml_diff>